<commit_message>
MA1101: Archivo de seguimiento de producción digital
</commit_message>
<xml_diff>
--- a/seguimiento/ProduccionDigital/SegDigital_MA_11_01_CO.xlsx
+++ b/seguimiento/ProduccionDigital/SegDigital_MA_11_01_CO.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -408,6 +408,18 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -416,18 +428,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -713,13 +713,13 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B7" sqref="B7"/>
+      <selection pane="topRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="7.796875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="46" style="1" customWidth="1"/>
+    <col min="2" max="2" width="56.265625" style="1" customWidth="1"/>
     <col min="3" max="3" width="10.53125" style="1" customWidth="1"/>
     <col min="4" max="4" width="8.3984375" style="1" customWidth="1"/>
     <col min="5" max="7" width="12.06640625" style="1" customWidth="1"/>
@@ -735,13 +735,13 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="G2" s="17" t="s">
+      <c r="G2" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="19"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="16"/>
     </row>
     <row r="3" spans="1:14" s="2" customFormat="1" ht="21.15" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
@@ -762,19 +762,19 @@
       <c r="F3" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="G3" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="H3" s="16" t="s">
+      <c r="H3" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="16" t="s">
+      <c r="I3" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="J3" s="16" t="s">
+      <c r="J3" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="K3" s="16" t="s">
+      <c r="K3" s="13" t="s">
         <v>35</v>
       </c>
       <c r="L3" s="6" t="s">
@@ -784,24 +784,26 @@
       <c r="N3" s="3"/>
     </row>
     <row r="4" spans="1:14" ht="15.85" x14ac:dyDescent="0.45">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="13"/>
+      <c r="B4" s="17"/>
       <c r="C4" s="7"/>
       <c r="D4" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="15">
+      <c r="E4" s="19">
         <v>42088.59375</v>
       </c>
-      <c r="F4" s="15"/>
+      <c r="F4" s="19">
+        <v>42090.680555555555</v>
+      </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="15"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="19"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A5" s="10" t="s">
@@ -816,14 +818,14 @@
       <c r="D5" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
       <c r="G5" s="9"/>
       <c r="H5" s="9"/>
       <c r="I5" s="9"/>
       <c r="J5" s="9"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="15"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="19"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A6" s="10" t="s">
@@ -838,14 +840,14 @@
       <c r="D6" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="15"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="19"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A7" s="10" t="s">
@@ -860,14 +862,14 @@
       <c r="D7" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="15"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="19"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A8" s="10" t="s">
@@ -882,14 +884,14 @@
       <c r="D8" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="15"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="19"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A9" s="10" t="s">
@@ -904,14 +906,14 @@
       <c r="D9" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
       <c r="J9" s="9"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="15"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="19"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A10" s="10" t="s">
@@ -926,14 +928,14 @@
       <c r="D10" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
       <c r="G10" s="9"/>
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="15"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="19"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A11" s="10" t="s">
@@ -948,14 +950,14 @@
       <c r="D11" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
       <c r="G11" s="9"/>
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
       <c r="J11" s="9"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="15"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="19"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A12" s="10" t="s">
@@ -970,16 +972,16 @@
       <c r="D12" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="15"/>
-    </row>
-    <row r="13" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="K12" s="18"/>
+      <c r="L12" s="19"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A13" s="10" t="s">
         <v>10</v>
       </c>
@@ -992,14 +994,14 @@
       <c r="D13" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="15"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="19"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A14" s="10" t="s">
@@ -1014,14 +1016,14 @@
       <c r="D14" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
       <c r="I14" s="9"/>
       <c r="J14" s="9"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="15"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="19"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A15" s="10" t="s">
@@ -1036,14 +1038,14 @@
       <c r="D15" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
       <c r="G15" s="9"/>
       <c r="H15" s="9"/>
       <c r="I15" s="9"/>
       <c r="J15" s="9"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="15"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="19"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A16" s="10" t="s">
@@ -1058,14 +1060,14 @@
       <c r="D16" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
       <c r="I16" s="9"/>
       <c r="J16" s="9"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="15"/>
+      <c r="K16" s="18"/>
+      <c r="L16" s="19"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A17" s="10" t="s">
@@ -1080,14 +1082,14 @@
       <c r="D17" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
       <c r="G17" s="9"/>
       <c r="H17" s="9"/>
       <c r="I17" s="9"/>
       <c r="J17" s="9"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="15"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="19"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A18" s="10" t="s">
@@ -1102,14 +1104,14 @@
       <c r="D18" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>
       <c r="I18" s="9"/>
       <c r="J18" s="9"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="15"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="19"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A19" s="10" t="s">
@@ -1124,16 +1126,16 @@
       <c r="D19" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
       <c r="G19" s="9"/>
       <c r="H19" s="9"/>
       <c r="I19" s="9"/>
       <c r="J19" s="9"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="15"/>
-    </row>
-    <row r="20" spans="1:12" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="K19" s="18"/>
+      <c r="L19" s="19"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A20" s="10" t="s">
         <v>17</v>
       </c>
@@ -1146,16 +1148,16 @@
       <c r="D20" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
       <c r="G20" s="9"/>
       <c r="H20" s="9"/>
       <c r="I20" s="9"/>
       <c r="J20" s="9"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="15"/>
-    </row>
-    <row r="21" spans="1:12" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="K20" s="18"/>
+      <c r="L20" s="19"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A21" s="10" t="s">
         <v>18</v>
       </c>
@@ -1168,14 +1170,14 @@
       <c r="D21" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
       <c r="G21" s="9"/>
       <c r="H21" s="9"/>
       <c r="I21" s="9"/>
       <c r="J21" s="9"/>
-      <c r="K21" s="14"/>
-      <c r="L21" s="15"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="19"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A22" s="10" t="s">
@@ -1190,14 +1192,14 @@
       <c r="D22" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
       <c r="G22" s="9"/>
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
       <c r="J22" s="9"/>
-      <c r="K22" s="14"/>
-      <c r="L22" s="15"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="19"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A23" s="10" t="s">
@@ -1212,14 +1214,14 @@
       <c r="D23" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
       <c r="G23" s="9"/>
       <c r="H23" s="9"/>
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
-      <c r="K23" s="14"/>
-      <c r="L23" s="15"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="19"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A24" s="10" t="s">
@@ -1234,14 +1236,14 @@
       <c r="D24" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
       <c r="G24" s="9"/>
       <c r="H24" s="9"/>
       <c r="I24" s="9"/>
       <c r="J24" s="9"/>
-      <c r="K24" s="14"/>
-      <c r="L24" s="15"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>